<commit_message>
update the fixture exporter
</commit_message>
<xml_diff>
--- a/fixtures/download_template/monitoring_data.xlsx
+++ b/fixtures/download_template/monitoring_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Level Measurement" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date and Time</t>
   </si>
   <si>
@@ -45,22 +42,16 @@
     <t xml:space="preserve">Method</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference elevation</t>
-  </si>
-  <si>
     <t xml:space="preserve">The original ID of the groundwater point.</t>
   </si>
   <si>
-    <t xml:space="preserve">3-letters ISO code of the country.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The date and time of the measurement or sampling.</t>
   </si>
   <si>
     <t xml:space="preserve">One of the following:
-• GWL_ASL ǀ Water level (elevation a.m.s.l.)
-• GWL_D ǀ Water level (depth)
-</t>
+• Water depth [from the ground surface]
+• Water depth [from the top of the well]
+• Water level elevation a.m.s.l.</t>
   </si>
   <si>
     <t xml:space="preserve">The value of the parameter.</t>
@@ -72,11 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">Explain the methodology used to collect the data, in the field and eventually in the lab.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only for water level depth measurements: What reference elevation the water level was measured? 
-• Ground ǀ Ground surface elevation
-• Top ǀ Elevation of the top of the casing</t>
   </si>
 </sst>
 </file>
@@ -308,26 +294,25 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="4" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -342,38 +327,30 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -392,26 +369,25 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="4" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -426,38 +402,30 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -476,26 +444,25 @@
     <tabColor rgb="FF953735"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="4" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -510,38 +477,30 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="159.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update permission for uploader and downloader
</commit_message>
<xml_diff>
--- a/fixtures/download_template/monitoring_data.xlsx
+++ b/fixtures/download_template/monitoring_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -59,10 +59,15 @@
   <si>
     <t xml:space="preserve">Unit must be either:
 • meter
+• feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the methodology used to collect the data, in the field and eventually in the lab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit must be either:
+• meter
 • foot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explain the methodology used to collect the data, in the field and eventually in the lab.</t>
   </si>
 </sst>
 </file>
@@ -297,7 +302,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,7 +424,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -494,7 +499,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>

</xml_diff>